<commit_message>
Added full support for (2D) non-energy descriptors. New pesky format issues have been introduced, though.
</commit_message>
<xml_diff>
--- a/test_files/aryl_ether_cleavage.xlsx
+++ b/test_files/aryl_ether_cleavage.xlsx
@@ -37,7 +37,7 @@
     <t xml:space="preserve">TS3</t>
   </si>
   <si>
-    <t xml:space="preserve">P</t>
+    <t xml:space="preserve">Product</t>
   </si>
   <si>
     <t xml:space="preserve">Ni(PMe3)</t>
@@ -210,10 +210,10 @@
   <dimension ref="A1:J22"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="88" zoomScaleNormal="88" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A22" activeCellId="0" sqref="A22:J22"/>
+      <selection pane="topLeft" activeCell="J1" activeCellId="0" sqref="J1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">

</xml_diff>

<commit_message>
Bugfixes and extra datasets.
</commit_message>
<xml_diff>
--- a/test_files/aryl_ether_cleavage.xlsx
+++ b/test_files/aryl_ether_cleavage.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t xml:space="preserve">Catalyst</t>
   </si>
@@ -28,10 +28,22 @@
     <t xml:space="preserve">R</t>
   </si>
   <si>
-    <t xml:space="preserve">TS1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TS2</t>
+    <t xml:space="preserve">ΔGRRS(2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ΔGRRS(TS1)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ΔGRRS(3)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ΔGRRS(TS2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ΔGRRS(4)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ΔGRRS(5)</t>
   </si>
   <si>
     <t xml:space="preserve">TS3</t>
@@ -181,13 +193,17 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -210,10 +226,10 @@
   <dimension ref="A1:J22"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="88" zoomScaleNormal="88" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J1" activeCellId="0" sqref="J1"/>
+      <selection pane="topLeft" activeCell="I1" activeCellId="0" sqref="I1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -222,700 +238,700 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="n">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="0" t="n">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" s="0" t="n">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="0" t="n">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="J1" s="0" t="s">
-        <v>5</v>
+      <c r="G1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="B2" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="C2" s="0" t="n">
+      <c r="C2" s="2" t="n">
         <v>0.25</v>
       </c>
-      <c r="D2" s="0" t="n">
+      <c r="D2" s="2" t="n">
         <v>27.36</v>
       </c>
-      <c r="E2" s="0" t="n">
+      <c r="E2" s="2" t="n">
         <v>10.5</v>
       </c>
-      <c r="F2" s="0" t="n">
+      <c r="F2" s="2" t="n">
         <v>23.87</v>
       </c>
-      <c r="G2" s="0" t="n">
+      <c r="G2" s="2" t="n">
         <v>-19.87</v>
       </c>
-      <c r="H2" s="0" t="n">
+      <c r="H2" s="2" t="n">
         <v>-27.54</v>
       </c>
-      <c r="I2" s="0" t="n">
+      <c r="I2" s="2" t="n">
         <v>-0.51</v>
       </c>
-      <c r="J2" s="0" t="n">
+      <c r="J2" s="2" t="n">
         <v>-28.1</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="B3" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="C3" s="0" t="n">
+      <c r="C3" s="2" t="n">
         <v>0.33</v>
       </c>
-      <c r="D3" s="0" t="n">
+      <c r="D3" s="2" t="n">
         <v>23.12</v>
       </c>
-      <c r="E3" s="0" t="n">
+      <c r="E3" s="2" t="n">
         <v>5.49</v>
       </c>
-      <c r="F3" s="0" t="n">
+      <c r="F3" s="2" t="n">
         <v>15.82</v>
       </c>
-      <c r="G3" s="0" t="n">
+      <c r="G3" s="2" t="n">
         <v>-26.18</v>
       </c>
-      <c r="H3" s="0" t="n">
+      <c r="H3" s="2" t="n">
         <v>-36.56</v>
       </c>
-      <c r="I3" s="0" t="n">
+      <c r="I3" s="2" t="n">
         <v>-5.78</v>
       </c>
-      <c r="J3" s="0" t="n">
+      <c r="J3" s="2" t="n">
         <v>-28.1</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="B4" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="C4" s="0" t="n">
+      <c r="C4" s="2" t="n">
         <v>9.34</v>
       </c>
-      <c r="D4" s="0" t="n">
+      <c r="D4" s="2" t="n">
         <v>32.06</v>
       </c>
-      <c r="E4" s="0" t="n">
+      <c r="E4" s="2" t="n">
         <v>17.55</v>
       </c>
-      <c r="F4" s="0" t="n">
+      <c r="F4" s="2" t="n">
         <v>27.98</v>
       </c>
-      <c r="G4" s="0" t="n">
+      <c r="G4" s="2" t="n">
         <v>-12</v>
       </c>
-      <c r="H4" s="0" t="n">
+      <c r="H4" s="2" t="n">
         <v>-27.89</v>
       </c>
-      <c r="I4" s="0" t="n">
+      <c r="I4" s="2" t="n">
         <v>4.69</v>
       </c>
-      <c r="J4" s="0" t="n">
+      <c r="J4" s="2" t="n">
         <v>-28.1</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B5" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="C5" s="0" t="n">
+      <c r="C5" s="2" t="n">
         <v>2.27</v>
       </c>
-      <c r="D5" s="0" t="n">
+      <c r="D5" s="2" t="n">
         <v>31.11</v>
       </c>
-      <c r="E5" s="0" t="n">
+      <c r="E5" s="2" t="n">
         <v>13.68</v>
       </c>
-      <c r="F5" s="0" t="n">
+      <c r="F5" s="2" t="n">
         <v>27.27</v>
       </c>
-      <c r="G5" s="0" t="n">
+      <c r="G5" s="2" t="n">
         <v>-16.89</v>
       </c>
-      <c r="H5" s="0" t="n">
+      <c r="H5" s="2" t="n">
         <v>-24.94</v>
       </c>
-      <c r="I5" s="0" t="n">
+      <c r="I5" s="2" t="n">
         <v>5.3</v>
       </c>
-      <c r="J5" s="0" t="n">
+      <c r="J5" s="2" t="n">
         <v>-28.1</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="B6" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="C6" s="0" t="n">
+      <c r="C6" s="2" t="n">
         <v>-7.45</v>
       </c>
-      <c r="D6" s="0" t="n">
+      <c r="D6" s="2" t="n">
         <v>17.57</v>
       </c>
-      <c r="E6" s="0" t="n">
+      <c r="E6" s="2" t="n">
         <v>-7.21</v>
       </c>
-      <c r="F6" s="0" t="n">
+      <c r="F6" s="2" t="n">
         <v>5.16</v>
       </c>
-      <c r="G6" s="0" t="n">
+      <c r="G6" s="2" t="n">
         <v>-35.81</v>
       </c>
-      <c r="H6" s="0" t="n">
+      <c r="H6" s="2" t="n">
         <v>-37.19</v>
       </c>
-      <c r="I6" s="0" t="n">
+      <c r="I6" s="2" t="n">
         <v>-15.95</v>
       </c>
-      <c r="J6" s="0" t="n">
+      <c r="J6" s="2" t="n">
         <v>-28.1</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="B7" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="C7" s="0" t="n">
+      <c r="C7" s="2" t="n">
         <v>4.68</v>
       </c>
-      <c r="D7" s="0" t="n">
+      <c r="D7" s="2" t="n">
         <v>27.95</v>
       </c>
-      <c r="E7" s="0" t="n">
+      <c r="E7" s="2" t="n">
         <v>13.85</v>
       </c>
-      <c r="F7" s="0" t="n">
+      <c r="F7" s="2" t="n">
         <v>25.95</v>
       </c>
-      <c r="G7" s="0" t="n">
+      <c r="G7" s="2" t="n">
         <v>-14.93</v>
       </c>
-      <c r="H7" s="0" t="n">
+      <c r="H7" s="2" t="n">
         <v>-24.8</v>
       </c>
-      <c r="I7" s="0" t="n">
+      <c r="I7" s="2" t="n">
         <v>2.07</v>
       </c>
-      <c r="J7" s="0" t="n">
+      <c r="J7" s="2" t="n">
         <v>-28.1</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="B8" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="C8" s="0" t="n">
+      <c r="C8" s="2" t="n">
         <v>-9.11</v>
       </c>
-      <c r="D8" s="0" t="n">
+      <c r="D8" s="2" t="n">
         <v>20.38</v>
       </c>
-      <c r="E8" s="0" t="n">
+      <c r="E8" s="2" t="n">
         <v>4.94</v>
       </c>
-      <c r="F8" s="0" t="n">
+      <c r="F8" s="2" t="n">
         <v>26.25</v>
       </c>
-      <c r="G8" s="0" t="n">
+      <c r="G8" s="2" t="n">
         <v>-30.63</v>
       </c>
-      <c r="H8" s="0" t="n">
+      <c r="H8" s="2" t="n">
         <v>-26.14</v>
       </c>
-      <c r="I8" s="0" t="n">
+      <c r="I8" s="2" t="n">
         <v>-5.09</v>
       </c>
-      <c r="J8" s="0" t="n">
+      <c r="J8" s="2" t="n">
         <v>-28.1</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="B9" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="C9" s="0" t="n">
+      <c r="C9" s="2" t="n">
         <v>-7.95</v>
       </c>
-      <c r="D9" s="0" t="n">
+      <c r="D9" s="2" t="n">
         <v>19.51</v>
       </c>
-      <c r="E9" s="0" t="n">
+      <c r="E9" s="2" t="n">
         <v>2.65</v>
       </c>
-      <c r="F9" s="0" t="n">
+      <c r="F9" s="2" t="n">
         <v>17.76</v>
       </c>
-      <c r="G9" s="0" t="n">
+      <c r="G9" s="2" t="n">
         <v>-27.96</v>
       </c>
-      <c r="H9" s="0" t="n">
+      <c r="H9" s="2" t="n">
         <v>-28.69</v>
       </c>
-      <c r="I9" s="0" t="n">
+      <c r="I9" s="2" t="n">
         <v>-5.39</v>
       </c>
-      <c r="J9" s="0" t="n">
+      <c r="J9" s="2" t="n">
         <v>-28.1</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="B10" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="C10" s="0" t="n">
+      <c r="C10" s="2" t="n">
         <v>4.1</v>
       </c>
-      <c r="D10" s="0" t="n">
+      <c r="D10" s="2" t="n">
         <v>26.65</v>
       </c>
-      <c r="E10" s="0" t="n">
+      <c r="E10" s="2" t="n">
         <v>8.02</v>
       </c>
-      <c r="F10" s="0" t="n">
+      <c r="F10" s="2" t="n">
         <v>19.63</v>
       </c>
-      <c r="G10" s="0" t="n">
+      <c r="G10" s="2" t="n">
         <v>-23.9</v>
       </c>
-      <c r="H10" s="0" t="n">
+      <c r="H10" s="2" t="n">
         <v>-41.03</v>
       </c>
-      <c r="I10" s="0" t="n">
+      <c r="I10" s="2" t="n">
         <v>-4.96</v>
       </c>
-      <c r="J10" s="0" t="n">
+      <c r="J10" s="2" t="n">
         <v>-28.1</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="B11" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="C11" s="0" t="n">
+      <c r="C11" s="2" t="n">
         <v>6.34</v>
       </c>
-      <c r="D11" s="0" t="n">
+      <c r="D11" s="2" t="n">
         <v>28.6</v>
       </c>
-      <c r="E11" s="0" t="n">
+      <c r="E11" s="2" t="n">
         <v>11.42</v>
       </c>
-      <c r="F11" s="0" t="n">
+      <c r="F11" s="2" t="n">
         <v>22.81</v>
       </c>
-      <c r="G11" s="0" t="n">
+      <c r="G11" s="2" t="n">
         <v>-17.96</v>
       </c>
-      <c r="H11" s="0" t="n">
+      <c r="H11" s="2" t="n">
         <v>-40.31</v>
       </c>
-      <c r="I11" s="0" t="n">
+      <c r="I11" s="2" t="n">
         <v>-0.07</v>
       </c>
-      <c r="J11" s="0" t="n">
+      <c r="J11" s="2" t="n">
         <v>-28.1</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="B12" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="C12" s="0" t="n">
+      <c r="C12" s="2" t="n">
         <v>-28.55</v>
       </c>
-      <c r="D12" s="0" t="n">
+      <c r="D12" s="2" t="n">
         <v>8.7</v>
       </c>
-      <c r="E12" s="0" t="n">
+      <c r="E12" s="2" t="n">
         <v>-19.49</v>
       </c>
-      <c r="F12" s="0" t="n">
+      <c r="F12" s="2" t="n">
         <v>-5.96</v>
       </c>
-      <c r="G12" s="0" t="n">
+      <c r="G12" s="2" t="n">
         <v>-52.45</v>
       </c>
-      <c r="H12" s="0" t="n">
+      <c r="H12" s="2" t="n">
         <v>-49.63</v>
       </c>
-      <c r="I12" s="0" t="n">
+      <c r="I12" s="2" t="n">
         <v>-24.87</v>
       </c>
-      <c r="J12" s="0" t="n">
+      <c r="J12" s="2" t="n">
         <v>-28.1</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="B13" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="C13" s="0" t="n">
+      <c r="C13" s="2" t="n">
         <v>-37.4</v>
       </c>
-      <c r="D13" s="0" t="n">
+      <c r="D13" s="2" t="n">
         <v>-0.71</v>
       </c>
-      <c r="E13" s="0" t="n">
+      <c r="E13" s="2" t="n">
         <v>-22.35</v>
       </c>
-      <c r="F13" s="0" t="n">
+      <c r="F13" s="2" t="n">
         <v>-11.93</v>
       </c>
-      <c r="G13" s="0" t="n">
+      <c r="G13" s="2" t="n">
         <v>-54.68</v>
       </c>
-      <c r="H13" s="0" t="n">
+      <c r="H13" s="2" t="n">
         <v>-60.93</v>
       </c>
-      <c r="I13" s="0" t="n">
+      <c r="I13" s="2" t="n">
         <v>-40.26</v>
       </c>
-      <c r="J13" s="0" t="n">
+      <c r="J13" s="2" t="n">
         <v>-28.1</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="B14" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="C14" s="0" t="n">
+      <c r="C14" s="2" t="n">
         <v>-37.79</v>
       </c>
-      <c r="D14" s="0" t="n">
+      <c r="D14" s="2" t="n">
         <v>-6.21</v>
       </c>
-      <c r="E14" s="0" t="n">
+      <c r="E14" s="2" t="n">
         <v>-30.28</v>
       </c>
-      <c r="F14" s="0" t="n">
+      <c r="F14" s="2" t="n">
         <v>-19.35</v>
       </c>
-      <c r="G14" s="0" t="n">
+      <c r="G14" s="2" t="n">
         <v>-67.38</v>
       </c>
-      <c r="H14" s="0" t="n">
+      <c r="H14" s="2" t="n">
         <v>-61.66</v>
       </c>
-      <c r="I14" s="0" t="n">
+      <c r="I14" s="2" t="n">
         <v>-38.82</v>
       </c>
-      <c r="J14" s="0" t="n">
+      <c r="J14" s="2" t="n">
         <v>-28.1</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="B15" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="C15" s="0" t="n">
+      <c r="C15" s="2" t="n">
         <v>-4.79</v>
       </c>
-      <c r="D15" s="0" t="n">
+      <c r="D15" s="2" t="n">
         <v>25.03</v>
       </c>
-      <c r="E15" s="0" t="n">
+      <c r="E15" s="2" t="n">
         <v>7.02</v>
       </c>
-      <c r="F15" s="0" t="n">
+      <c r="F15" s="2" t="n">
         <v>19.01</v>
       </c>
-      <c r="G15" s="0" t="n">
+      <c r="G15" s="2" t="n">
         <v>-24.95</v>
       </c>
-      <c r="H15" s="0" t="n">
+      <c r="H15" s="2" t="n">
         <v>-34.25</v>
       </c>
-      <c r="I15" s="0" t="n">
+      <c r="I15" s="2" t="n">
         <v>-8.95</v>
       </c>
-      <c r="J15" s="0" t="n">
+      <c r="J15" s="2" t="n">
         <v>-28.1</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="B16" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="C16" s="0" t="n">
+      <c r="C16" s="2" t="n">
         <v>-3.78</v>
       </c>
-      <c r="D16" s="0" t="n">
+      <c r="D16" s="2" t="n">
         <v>23.8</v>
       </c>
-      <c r="E16" s="0" t="n">
+      <c r="E16" s="2" t="n">
         <v>10.72</v>
       </c>
-      <c r="F16" s="0" t="n">
+      <c r="F16" s="2" t="n">
         <v>25.18</v>
       </c>
-      <c r="G16" s="0" t="n">
+      <c r="G16" s="2" t="n">
         <v>-24.12</v>
       </c>
-      <c r="H16" s="0" t="n">
+      <c r="H16" s="2" t="n">
         <v>-32.67</v>
       </c>
-      <c r="I16" s="0" t="n">
+      <c r="I16" s="2" t="n">
         <v>-8.95</v>
       </c>
-      <c r="J16" s="0" t="n">
+      <c r="J16" s="2" t="n">
         <v>-28.1</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="B17" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="C17" s="0" t="n">
+      <c r="C17" s="2" t="n">
         <v>7.9</v>
       </c>
-      <c r="D17" s="0" t="n">
+      <c r="D17" s="2" t="n">
         <v>36.07</v>
       </c>
-      <c r="E17" s="0" t="n">
+      <c r="E17" s="2" t="n">
         <v>18.3</v>
       </c>
-      <c r="F17" s="0" t="n">
+      <c r="F17" s="2" t="n">
         <v>30.84</v>
       </c>
-      <c r="G17" s="0" t="n">
+      <c r="G17" s="2" t="n">
         <v>-13.1</v>
       </c>
-      <c r="H17" s="0" t="n">
+      <c r="H17" s="2" t="n">
         <v>-28.65</v>
       </c>
-      <c r="I17" s="0" t="n">
+      <c r="I17" s="2" t="n">
         <v>6.01</v>
       </c>
-      <c r="J17" s="0" t="n">
+      <c r="J17" s="2" t="n">
         <v>-28.1</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="B18" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="C18" s="0" t="n">
+      <c r="C18" s="2" t="n">
         <v>9.15</v>
       </c>
-      <c r="D18" s="0" t="n">
+      <c r="D18" s="2" t="n">
         <v>38.11</v>
       </c>
-      <c r="E18" s="0" t="n">
+      <c r="E18" s="2" t="n">
         <v>20.12</v>
       </c>
-      <c r="F18" s="0" t="n">
+      <c r="F18" s="2" t="n">
         <v>32.21</v>
       </c>
-      <c r="G18" s="0" t="n">
+      <c r="G18" s="2" t="n">
         <v>-8.77</v>
       </c>
-      <c r="H18" s="0" t="n">
+      <c r="H18" s="2" t="n">
         <v>-27.11</v>
       </c>
-      <c r="I18" s="0" t="n">
+      <c r="I18" s="2" t="n">
         <v>8.18</v>
       </c>
-      <c r="J18" s="0" t="n">
+      <c r="J18" s="2" t="n">
         <v>-28.1</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="B19" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="C19" s="0" t="n">
+      <c r="C19" s="2" t="n">
         <v>1.7</v>
       </c>
-      <c r="D19" s="0" t="n">
+      <c r="D19" s="2" t="n">
         <v>28.86</v>
       </c>
-      <c r="E19" s="0" t="n">
+      <c r="E19" s="2" t="n">
         <v>13.22</v>
       </c>
-      <c r="F19" s="0" t="n">
+      <c r="F19" s="2" t="n">
         <v>26.87</v>
       </c>
-      <c r="G19" s="0" t="n">
+      <c r="G19" s="2" t="n">
         <v>-17.28</v>
       </c>
-      <c r="H19" s="0" t="n">
+      <c r="H19" s="2" t="n">
         <v>-27.23</v>
       </c>
-      <c r="I19" s="0" t="n">
+      <c r="I19" s="2" t="n">
         <v>0.81</v>
       </c>
-      <c r="J19" s="0" t="n">
+      <c r="J19" s="2" t="n">
         <v>-28.1</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="B20" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="C20" s="0" t="n">
+      <c r="C20" s="2" t="n">
         <v>5.05</v>
       </c>
-      <c r="D20" s="0" t="n">
+      <c r="D20" s="2" t="n">
         <v>32.83</v>
       </c>
-      <c r="E20" s="0" t="n">
+      <c r="E20" s="2" t="n">
         <v>18.87</v>
       </c>
-      <c r="F20" s="0" t="n">
+      <c r="F20" s="2" t="n">
         <v>33.08</v>
       </c>
-      <c r="G20" s="0" t="n">
+      <c r="G20" s="2" t="n">
         <v>-12.75</v>
       </c>
-      <c r="H20" s="0" t="n">
+      <c r="H20" s="2" t="n">
         <v>-26.85</v>
       </c>
-      <c r="I20" s="0" t="n">
+      <c r="I20" s="2" t="n">
         <v>6.58</v>
       </c>
-      <c r="J20" s="0" t="n">
+      <c r="J20" s="2" t="n">
         <v>-28.1</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="B21" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="C21" s="0" t="n">
+      <c r="C21" s="2" t="n">
         <v>6.01</v>
       </c>
-      <c r="D21" s="0" t="n">
+      <c r="D21" s="2" t="n">
         <v>30.99</v>
       </c>
-      <c r="E21" s="0" t="n">
+      <c r="E21" s="2" t="n">
         <v>13.55</v>
       </c>
-      <c r="F21" s="0" t="n">
+      <c r="F21" s="2" t="n">
         <v>27.22</v>
       </c>
-      <c r="G21" s="0" t="n">
+      <c r="G21" s="2" t="n">
         <v>-13.9</v>
       </c>
-      <c r="H21" s="0" t="n">
+      <c r="H21" s="2" t="n">
         <v>-29.7</v>
       </c>
-      <c r="I21" s="0" t="n">
+      <c r="I21" s="2" t="n">
         <v>5.06</v>
       </c>
-      <c r="J21" s="0" t="n">
+      <c r="J21" s="2" t="n">
         <v>-28.1</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="B22" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="C22" s="0" t="n">
+      <c r="C22" s="2" t="n">
         <v>-0.02</v>
       </c>
-      <c r="D22" s="0" t="n">
+      <c r="D22" s="2" t="n">
         <v>26.44</v>
       </c>
-      <c r="E22" s="0" t="n">
+      <c r="E22" s="2" t="n">
         <v>5.71</v>
       </c>
-      <c r="F22" s="0" t="n">
+      <c r="F22" s="2" t="n">
         <v>15.02</v>
       </c>
-      <c r="G22" s="0" t="n">
+      <c r="G22" s="2" t="n">
         <v>-25.48</v>
       </c>
-      <c r="H22" s="0" t="n">
+      <c r="H22" s="2" t="n">
         <v>-29.13</v>
       </c>
-      <c r="I22" s="0" t="n">
+      <c r="I22" s="2" t="n">
         <v>-3.93</v>
       </c>
-      <c r="J22" s="0" t="n">
+      <c r="J22" s="2" t="n">
         <v>-28.1</v>
       </c>
     </row>

</xml_diff>